<commit_message>
Commit TestRound 1&2 và TestReport
</commit_message>
<xml_diff>
--- a/WIP/Deliverable/Report5/VMN_Test Report_v1.1_EN.xlsx
+++ b/WIP/Deliverable/Report5/VMN_Test Report_v1.1_EN.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26722"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26505"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Romeo/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27320" windowHeight="12420" activeTab="1"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="25520" windowHeight="15540" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="2" r:id="rId1"/>
@@ -23,7 +28,7 @@
     <definedName name="Title">"$#REF!.$C$14"</definedName>
     <definedName name="Version">"$#REF!.$N$16"</definedName>
   </definedNames>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -70,7 +75,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="64">
   <si>
     <t>Quality Management System</t>
   </si>
@@ -126,9 +131,6 @@
     <t>Version : 1.0</t>
   </si>
   <si>
-    <t>PM</t>
-  </si>
-  <si>
     <t>Create document</t>
   </si>
   <si>
@@ -207,70 +209,64 @@
     <t>Defect report</t>
   </si>
   <si>
-    <t>Round 3</t>
-  </si>
-  <si>
-    <t>DDL</t>
-  </si>
-  <si>
-    <t>DDL_Test Report</t>
-  </si>
-  <si>
-    <t>Cao Thị Phương Mai</t>
-  </si>
-  <si>
-    <t>Lưu Ngọc Mạnh</t>
-  </si>
-  <si>
-    <t>Vũ Công Chính</t>
-  </si>
-  <si>
     <t>Member</t>
   </si>
   <si>
-    <t>40TC/KLOC</t>
-  </si>
-  <si>
-    <t>30TC/KLOC</t>
-  </si>
-  <si>
-    <t>20TC/KLOC</t>
-  </si>
-  <si>
     <t>Acceptance Test</t>
   </si>
   <si>
     <t>N/A</t>
   </si>
   <si>
-    <t>3 -4 defects/KLOC</t>
-  </si>
-  <si>
-    <t>2 -3 defects/KLOC</t>
-  </si>
-  <si>
-    <t>4 -6 defects/KLOC</t>
-  </si>
-  <si>
-    <t>1-2 defects/KLOC</t>
-  </si>
-  <si>
-    <t>10-15 defects/KLOC</t>
-  </si>
-  <si>
-    <t>90TC/KLOC</t>
-  </si>
-  <si>
-    <t>1 defects/KLOC</t>
-  </si>
-  <si>
-    <t>9 defects/KLOC</t>
-  </si>
-  <si>
-    <t>2 defects/KLOC</t>
-  </si>
-  <si>
-    <t>12 defects/KLOC</t>
+    <t>10TC/function</t>
+  </si>
+  <si>
+    <t>2 -3 defects/function</t>
+  </si>
+  <si>
+    <t>3 -4 defects/function</t>
+  </si>
+  <si>
+    <t>20TC/function</t>
+  </si>
+  <si>
+    <t>4 -6 defects/function</t>
+  </si>
+  <si>
+    <t>1-2 defects/function</t>
+  </si>
+  <si>
+    <t>10-15 defects/function</t>
+  </si>
+  <si>
+    <t>1 defects/function</t>
+  </si>
+  <si>
+    <t>9 defects/function</t>
+  </si>
+  <si>
+    <t>2 defects/function</t>
+  </si>
+  <si>
+    <t>12 defects/function</t>
+  </si>
+  <si>
+    <t>50TC/function</t>
+  </si>
+  <si>
+    <t>VMN</t>
+  </si>
+  <si>
+    <t>VMN_Test Report</t>
+  </si>
+  <si>
+    <t>Trần Bình Khánh</t>
+  </si>
+  <si>
+    <t>Hoàng Thị Quỳnh</t>
+  </si>
+  <si>
+    <t>Test Leader</t>
   </si>
 </sst>
 </file>
@@ -888,7 +884,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="95">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1038,15 +1034,6 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1074,9 +1061,6 @@
     <xf numFmtId="14" fontId="7" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1084,11 +1068,26 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1435,7 +1434,7 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
             <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
@@ -1477,7 +1476,7 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
             <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
@@ -1495,7 +1494,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1508,11 +1507,11 @@
   </sheetPr>
   <dimension ref="B1:F26"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="1.1640625" customWidth="1"/>
     <col min="2" max="2" width="20.83203125" customWidth="1"/>
@@ -1521,32 +1520,32 @@
     <col min="5" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:6" ht="38.25" customHeight="1">
+    <row r="1" spans="2:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="8"/>
-      <c r="C1" s="85" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="85"/>
-      <c r="E1" s="85"/>
-    </row>
-    <row r="2" spans="2:6" ht="30.75" customHeight="1">
-      <c r="B2" s="86" t="s">
-        <v>47</v>
-      </c>
-      <c r="C2" s="86"/>
-      <c r="D2" s="86"/>
-      <c r="E2" s="86"/>
-    </row>
-    <row r="3" spans="2:6" ht="20.25" customHeight="1">
+      <c r="C1" s="86" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+    </row>
+    <row r="2" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B2" s="87" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+    </row>
+    <row r="3" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="9"/>
       <c r="C3" s="9"/>
       <c r="D3" s="10"/>
       <c r="E3" s="11" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" spans="2:6" ht="16.5" customHeight="1">
+    <row r="4" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="13"/>
@@ -1555,98 +1554,98 @@
       </c>
       <c r="F4" s="13"/>
     </row>
-    <row r="5" spans="2:6" ht="16.5" customHeight="1">
+    <row r="5" spans="2:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
       <c r="D5" s="13"/>
       <c r="E5" s="15"/>
       <c r="F5" s="13"/>
     </row>
-    <row r="6" spans="2:6" s="1" customFormat="1" ht="18.75" customHeight="1">
-      <c r="B6" s="87" t="s">
+    <row r="6" spans="2:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="88" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="87"/>
-      <c r="D6" s="87"/>
-      <c r="E6" s="87"/>
-    </row>
-    <row r="7" spans="2:6" s="1" customFormat="1" ht="14.25" customHeight="1">
+      <c r="C6" s="88"/>
+      <c r="D6" s="88"/>
+      <c r="E6" s="88"/>
+    </row>
+    <row r="7" spans="2:6" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="88">
-        <v>42259</v>
-      </c>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-    </row>
-    <row r="8" spans="2:6" s="1" customFormat="1" ht="16.5" customHeight="1">
+      <c r="C7" s="89">
+        <v>42460</v>
+      </c>
+      <c r="D7" s="83"/>
+      <c r="E7" s="83"/>
+    </row>
+    <row r="8" spans="2:6" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="82" t="s">
+      <c r="C8" s="83" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="82"/>
-      <c r="E8" s="82"/>
-    </row>
-    <row r="9" spans="2:6" s="1" customFormat="1" ht="15" customHeight="1">
+      <c r="D8" s="83"/>
+      <c r="E8" s="83"/>
+    </row>
+    <row r="9" spans="2:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="82" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="82"/>
-      <c r="E9" s="82"/>
-    </row>
-    <row r="10" spans="2:6" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B10" s="83"/>
-      <c r="C10" s="83"/>
-      <c r="D10" s="83"/>
-      <c r="E10" s="83"/>
-    </row>
-    <row r="11" spans="2:6" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B11" s="84" t="s">
+      <c r="C9" s="83" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+    </row>
+    <row r="10" spans="2:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="84"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="84"/>
+      <c r="E10" s="84"/>
+    </row>
+    <row r="11" spans="2:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="85" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="18" t="s">
-        <v>49</v>
+        <v>62</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>18</v>
+        <v>63</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:6" s="1" customFormat="1" ht="12.75" customHeight="1">
-      <c r="B12" s="84"/>
+    <row r="12" spans="2:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="85"/>
       <c r="C12" s="18"/>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
     </row>
-    <row r="13" spans="2:6" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1">
+    <row r="13" spans="2:6" s="1" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B13" s="17" t="s">
         <v>7</v>
       </c>
       <c r="C13" s="21" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="E13" s="23"/>
     </row>
-    <row r="14" spans="2:6" s="1" customFormat="1" ht="13.5" customHeight="1">
-      <c r="B14" s="79" t="s">
+    <row r="14" spans="2:6" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B14" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-    </row>
-    <row r="15" spans="2:6" s="1" customFormat="1" ht="13.5" customHeight="1">
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+    </row>
+    <row r="15" spans="2:6" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="24" t="s">
         <v>8</v>
       </c>
@@ -1660,65 +1659,65 @@
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:6" s="1" customFormat="1" ht="26.25" customHeight="1">
-      <c r="B16" s="72">
-        <v>42259</v>
+    <row r="16" spans="2:6" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B16" s="69">
+        <v>42460</v>
       </c>
       <c r="C16" s="35">
         <v>1</v>
       </c>
       <c r="D16" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" s="1" customFormat="1" ht="13" thickBot="1">
+        <v>18</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" s="1" customFormat="1" ht="14" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B17" s="2"/>
       <c r="C17" s="3"/>
       <c r="D17" s="4"/>
       <c r="E17" s="5"/>
     </row>
-    <row r="18" spans="2:6" ht="15">
+    <row r="18" spans="2:6" ht="16" x14ac:dyDescent="0.15">
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
     </row>
-    <row r="19" spans="2:6" ht="18" customHeight="1">
+    <row r="19" spans="2:6" ht="18" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B19" s="28"/>
       <c r="C19" s="29"/>
     </row>
-    <row r="20" spans="2:6" ht="17">
-      <c r="B20" s="80"/>
-      <c r="C20" s="80"/>
+    <row r="20" spans="2:6" ht="18" x14ac:dyDescent="0.2">
+      <c r="B20" s="81"/>
+      <c r="C20" s="81"/>
       <c r="D20" s="7"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
     </row>
-    <row r="21" spans="2:6" ht="20.25" customHeight="1">
+    <row r="21" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B21" s="31"/>
       <c r="C21" s="29"/>
       <c r="D21" s="32"/>
       <c r="E21" s="32"/>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B22" s="33"/>
       <c r="C22" s="33"/>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B23" s="33"/>
       <c r="C23" s="33"/>
     </row>
-    <row r="24" spans="2:6" ht="13">
+    <row r="24" spans="2:6" ht="14" x14ac:dyDescent="0.15">
       <c r="B24" s="31"/>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.15">
       <c r="B25" s="29"/>
       <c r="C25" s="29"/>
     </row>
-    <row r="26" spans="2:6">
-      <c r="B26" s="81"/>
-      <c r="C26" s="81"/>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.15">
+      <c r="B26" s="82"/>
+      <c r="C26" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="11">
@@ -1740,23 +1739,18 @@
     <oddFooter>&amp;LTMA confidential&amp;CTMA Solutions&amp;RPage &amp;P of &amp;N</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:N30"/>
+  <dimension ref="B2:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:N20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="1" customWidth="1"/>
     <col min="2" max="2" width="16.5" customWidth="1"/>
@@ -1767,39 +1761,39 @@
     <col min="7" max="7" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:14">
+    <row r="2" spans="2:10" x14ac:dyDescent="0.15">
       <c r="C2" s="6"/>
     </row>
-    <row r="3" spans="2:14" ht="18">
-      <c r="B3" s="94" t="s">
+    <row r="3" spans="2:10" ht="20" x14ac:dyDescent="0.2">
+      <c r="B3" s="95" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-    </row>
-    <row r="4" spans="2:14">
+      <c r="C3" s="95"/>
+      <c r="D3" s="95"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
+      <c r="H3" s="95"/>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.15">
       <c r="D4" s="36"/>
     </row>
-    <row r="6" spans="2:14" ht="13" thickBot="1"/>
-    <row r="7" spans="2:14" ht="23" thickBot="1">
+    <row r="6" spans="2:10" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="7" spans="2:10" ht="25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B7" s="49" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="49" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="49" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="49" t="s">
         <v>41</v>
       </c>
-      <c r="D7" s="49" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7" s="49" t="s">
+      <c r="F7" s="49" t="s">
         <v>42</v>
-      </c>
-      <c r="F7" s="49" t="s">
-        <v>43</v>
       </c>
       <c r="G7" s="39" t="s">
         <v>15</v>
@@ -1808,20 +1802,22 @@
         <v>16</v>
       </c>
       <c r="I7" s="49" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="2:14" ht="19.5" customHeight="1">
-      <c r="B8" s="65" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="59" t="s">
-        <v>52</v>
-      </c>
-      <c r="D8" s="60" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="55"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B8" s="62" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="77" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="55">
+        <v>453</v>
+      </c>
       <c r="F8" s="55"/>
       <c r="G8" s="37">
         <v>1</v>
@@ -1833,21 +1829,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:14" ht="21.75" customHeight="1">
-      <c r="B9" s="66" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="61" t="s">
-        <v>53</v>
-      </c>
-      <c r="D9" s="73" t="s">
-        <v>58</v>
+    <row r="9" spans="2:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B9" s="63" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="75" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="76" t="s">
+        <v>48</v>
       </c>
       <c r="E9" s="56">
-        <v>300</v>
+        <v>142</v>
       </c>
       <c r="F9" s="56" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="G9" s="40">
         <v>1</v>
@@ -1855,75 +1851,78 @@
       <c r="H9" s="42">
         <v>1</v>
       </c>
-      <c r="I9" s="74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="2:14" ht="23.25" customHeight="1">
-      <c r="B10" s="75" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="76" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" s="77" t="s">
-        <v>59</v>
+      <c r="I9" s="70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B10" s="71" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="78" t="s">
+        <v>50</v>
+      </c>
+      <c r="D10" s="79" t="s">
+        <v>51</v>
       </c>
       <c r="E10" s="57">
-        <v>812</v>
+        <v>662</v>
       </c>
       <c r="F10" s="57" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="78">
+        <v>55</v>
+      </c>
+      <c r="G10" s="73">
         <v>1</v>
       </c>
-      <c r="H10" s="78">
+      <c r="H10" s="73">
         <v>1</v>
       </c>
       <c r="I10" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="2:14" ht="23.25" customHeight="1">
-      <c r="B11" s="75" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="76" t="s">
+    <row r="11" spans="2:10" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B11" s="71" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="72" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="79" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="57" t="s">
+        <v>46</v>
+      </c>
+      <c r="F11" s="57" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="77" t="s">
-        <v>60</v>
-      </c>
-      <c r="E11" s="57" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="57" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="78">
+      <c r="G11" s="73">
         <v>1</v>
       </c>
-      <c r="H11" s="78">
+      <c r="H11" s="73">
         <v>1</v>
       </c>
       <c r="I11" s="51">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:14" ht="20.25" customHeight="1">
-      <c r="B12" s="64" t="s">
-        <v>37</v>
+    <row r="12" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B12" s="61" t="s">
+        <v>36</v>
       </c>
       <c r="C12" s="45" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D12" s="45" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="45"/>
+        <v>53</v>
+      </c>
+      <c r="E12" s="45">
+        <f>SUM(E8:E10)</f>
+        <v>1257</v>
+      </c>
       <c r="F12" s="45" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="G12" s="44">
         <v>1</v>
@@ -1935,259 +1934,290 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="2:14">
-      <c r="B15" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="89" t="s">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B15" s="93" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="90" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="91"/>
+      <c r="E15" s="91"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="90" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="90"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="89" t="s">
+      <c r="H15" s="91"/>
+      <c r="I15" s="91"/>
+      <c r="J15" s="92"/>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B16" s="94"/>
+      <c r="C16" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="H15" s="90"/>
-      <c r="I15" s="90"/>
-      <c r="J15" s="91"/>
-      <c r="K15" s="89" t="s">
-        <v>45</v>
-      </c>
-      <c r="L15" s="90"/>
-      <c r="M15" s="90"/>
-      <c r="N15" s="91"/>
-    </row>
-    <row r="16" spans="2:14">
-      <c r="B16" s="93"/>
-      <c r="C16" s="58" t="s">
+      <c r="D16" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="D16" s="58" t="s">
+      <c r="E16" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="58" t="s">
+      <c r="F16" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="58" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="58" t="s">
+        <v>35</v>
+      </c>
+      <c r="J16" s="58" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="18" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B17" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="57">
+        <v>453</v>
+      </c>
+      <c r="D17" s="57">
+        <v>0</v>
+      </c>
+      <c r="E17" s="57">
+        <v>0</v>
+      </c>
+      <c r="F17" s="57">
+        <v>0</v>
+      </c>
+      <c r="G17" s="57">
+        <v>453</v>
+      </c>
+      <c r="H17" s="57">
+        <v>0</v>
+      </c>
+      <c r="I17" s="57">
+        <v>0</v>
+      </c>
+      <c r="J17" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="21" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B18" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="57">
+        <v>142</v>
+      </c>
+      <c r="D18" s="57">
+        <v>0</v>
+      </c>
+      <c r="E18" s="57">
+        <v>0</v>
+      </c>
+      <c r="F18" s="57">
+        <v>0</v>
+      </c>
+      <c r="G18" s="57">
+        <v>142</v>
+      </c>
+      <c r="H18" s="57">
+        <v>0</v>
+      </c>
+      <c r="I18" s="57">
+        <v>0</v>
+      </c>
+      <c r="J18" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B19" s="54" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="57">
+        <v>470</v>
+      </c>
+      <c r="D19" s="57">
+        <v>192</v>
+      </c>
+      <c r="E19" s="57">
+        <v>0</v>
+      </c>
+      <c r="F19" s="57">
+        <v>0</v>
+      </c>
+      <c r="G19" s="57">
+        <v>662</v>
+      </c>
+      <c r="H19" s="57">
+        <v>0</v>
+      </c>
+      <c r="I19" s="57">
+        <v>0</v>
+      </c>
+      <c r="J19" s="57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B20" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="G16" s="58" t="s">
-        <v>34</v>
-      </c>
-      <c r="H16" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="I16" s="58" t="s">
-        <v>36</v>
-      </c>
-      <c r="J16" s="58" t="s">
-        <v>56</v>
-      </c>
-      <c r="K16" s="58" t="s">
-        <v>34</v>
-      </c>
-      <c r="L16" s="58" t="s">
-        <v>35</v>
-      </c>
-      <c r="M16" s="58" t="s">
-        <v>36</v>
-      </c>
-      <c r="N16" s="58" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="2:14" ht="18" customHeight="1">
-      <c r="B17" s="54" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="57"/>
-      <c r="D17" s="57"/>
-      <c r="E17" s="57"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="57"/>
-      <c r="I17" s="57"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
-      <c r="M17" s="57"/>
-      <c r="N17" s="57"/>
-    </row>
-    <row r="18" spans="2:14" ht="21" customHeight="1">
-      <c r="B18" s="54" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="57"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="57"/>
-      <c r="I18" s="57"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="57"/>
-      <c r="M18" s="57"/>
-      <c r="N18" s="57"/>
-    </row>
-    <row r="19" spans="2:14" ht="20.25" customHeight="1">
-      <c r="B19" s="54" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="57"/>
-      <c r="N19" s="57"/>
-    </row>
-    <row r="20" spans="2:14" ht="18.75" customHeight="1">
-      <c r="B20" s="43" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="45"/>
-      <c r="D20" s="45"/>
-      <c r="E20" s="45"/>
-      <c r="F20" s="45"/>
-      <c r="G20" s="45"/>
-      <c r="H20" s="45"/>
-      <c r="I20" s="45"/>
-      <c r="J20" s="45"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="57"/>
-      <c r="M20" s="57"/>
-      <c r="N20" s="57"/>
-    </row>
-    <row r="23" spans="2:14" ht="17">
-      <c r="B23" s="71" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="24" spans="2:14" ht="13" thickBot="1"/>
-    <row r="25" spans="2:14" ht="26.25" customHeight="1" thickBot="1">
+      <c r="C20" s="45">
+        <f t="shared" ref="C20:H20" si="0">SUM(C17:C19)</f>
+        <v>1065</v>
+      </c>
+      <c r="D20" s="45">
+        <f t="shared" si="0"/>
+        <v>192</v>
+      </c>
+      <c r="E20" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F20" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="45">
+        <f t="shared" si="0"/>
+        <v>1257</v>
+      </c>
+      <c r="H20" s="45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I20" s="45">
+        <v>0</v>
+      </c>
+      <c r="J20" s="45">
+        <f>SUM(J17:J19)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" ht="18" x14ac:dyDescent="0.2">
+      <c r="B23" s="68" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" ht="14" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="25" spans="2:10" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B25" s="53" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="D25" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="38" t="s">
+      <c r="E25" s="38" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="38" t="s">
+      <c r="F25" s="52" t="s">
         <v>22</v>
       </c>
-      <c r="F25" s="52" t="s">
+    </row>
+    <row r="26" spans="2:10" s="34" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B26" s="59" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="2:14" s="34" customFormat="1" ht="17.25" customHeight="1">
-      <c r="B26" s="62" t="s">
+      <c r="C26" s="64">
+        <v>0</v>
+      </c>
+      <c r="D26" s="65">
+        <v>0</v>
+      </c>
+      <c r="E26" s="65">
+        <v>0</v>
+      </c>
+      <c r="F26" s="65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B27" s="60" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="67">
-        <v>0</v>
-      </c>
-      <c r="D26" s="68">
-        <v>0</v>
-      </c>
-      <c r="E26" s="68">
-        <v>0</v>
-      </c>
-      <c r="F26" s="68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:14" ht="17.25" customHeight="1">
-      <c r="B27" s="63" t="s">
+      <c r="C27" s="66">
+        <v>3</v>
+      </c>
+      <c r="D27" s="65">
+        <v>0</v>
+      </c>
+      <c r="E27" s="65">
+        <v>0</v>
+      </c>
+      <c r="F27" s="65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B28" s="60" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="69">
-        <v>4</v>
-      </c>
-      <c r="D27" s="68">
-        <v>0</v>
-      </c>
-      <c r="E27" s="68">
-        <v>0</v>
-      </c>
-      <c r="F27" s="68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:14" ht="14.25" customHeight="1">
-      <c r="B28" s="63" t="s">
-        <v>26</v>
-      </c>
       <c r="C28" s="47">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="D28" s="37">
         <v>1</v>
       </c>
-      <c r="E28" s="68">
-        <v>0</v>
-      </c>
-      <c r="F28" s="68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:14" ht="13.5" customHeight="1">
-      <c r="B29" s="63" t="s">
-        <v>28</v>
+      <c r="E28" s="65">
+        <v>0</v>
+      </c>
+      <c r="F28" s="65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B29" s="60" t="s">
+        <v>27</v>
       </c>
       <c r="C29" s="48">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="D29" s="40">
         <v>1</v>
       </c>
-      <c r="E29" s="68">
-        <v>0</v>
-      </c>
-      <c r="F29" s="68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="2:14">
-      <c r="B30" s="64" t="s">
-        <v>37</v>
+      <c r="E29" s="65">
+        <v>0</v>
+      </c>
+      <c r="F29" s="65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.15">
+      <c r="B30" s="61" t="s">
+        <v>36</v>
       </c>
       <c r="C30" s="45">
-        <v>66</v>
+        <v>16</v>
       </c>
       <c r="D30" s="44">
         <v>1</v>
       </c>
-      <c r="E30" s="70">
-        <v>0</v>
-      </c>
-      <c r="F30" s="70">
+      <c r="E30" s="67">
+        <v>0</v>
+      </c>
+      <c r="F30" s="67">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="C15:F15"/>
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="G15:J15"/>
     <mergeCell ref="B3:H3"/>
-    <mergeCell ref="K15:N15"/>
   </mergeCells>
   <pageMargins left="0.74791666666666667" right="0.74791666666666667" top="0.98402777777777783" bottom="0.98402777777777783" header="0.51180555555555562" footer="0.51180555555555562"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit Test UnitTest và update
</commit_message>
<xml_diff>
--- a/WIP/Deliverable/Report5/VMN_Test Report_v1.1_EN.xlsx
+++ b/WIP/Deliverable/Report5/VMN_Test Report_v1.1_EN.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Romeo/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Romeo/Documents/201601JS01/WIP/Deliverable/Report5/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1089,6 +1089,21 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1098,25 +1113,10 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1522,19 +1522,19 @@
   <sheetData>
     <row r="1" spans="2:6" ht="38.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B1" s="8"/>
-      <c r="C1" s="86" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
+      <c r="C1" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
     </row>
     <row r="2" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="81" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
     </row>
     <row r="3" spans="2:6" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="9"/>
@@ -1562,51 +1562,51 @@
       <c r="F5" s="13"/>
     </row>
     <row r="6" spans="2:6" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B6" s="88" t="s">
+      <c r="B6" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="88"/>
-      <c r="D6" s="88"/>
-      <c r="E6" s="88"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
     </row>
     <row r="7" spans="2:6" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B7" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="89">
+      <c r="C7" s="83">
         <v>42460</v>
       </c>
-      <c r="D7" s="83"/>
-      <c r="E7" s="83"/>
+      <c r="D7" s="84"/>
+      <c r="E7" s="84"/>
     </row>
     <row r="8" spans="2:6" s="1" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="83" t="s">
+      <c r="C8" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="83"/>
-      <c r="E8" s="83"/>
+      <c r="D8" s="84"/>
+      <c r="E8" s="84"/>
     </row>
     <row r="9" spans="2:6" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="83" t="s">
+      <c r="C9" s="84" t="s">
         <v>61</v>
       </c>
-      <c r="D9" s="83"/>
-      <c r="E9" s="83"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
     </row>
     <row r="10" spans="2:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
+      <c r="B10" s="88"/>
+      <c r="C10" s="88"/>
+      <c r="D10" s="88"/>
+      <c r="E10" s="88"/>
     </row>
     <row r="11" spans="2:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="89" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="18" t="s">
@@ -1620,7 +1620,7 @@
       </c>
     </row>
     <row r="12" spans="2:6" s="1" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B12" s="85"/>
+      <c r="B12" s="89"/>
       <c r="C12" s="18"/>
       <c r="D12" s="19"/>
       <c r="E12" s="20"/>
@@ -1638,12 +1638,12 @@
       <c r="E13" s="23"/>
     </row>
     <row r="14" spans="2:6" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B14" s="80" t="s">
+      <c r="B14" s="85" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
+      <c r="C14" s="85"/>
+      <c r="D14" s="85"/>
+      <c r="E14" s="85"/>
     </row>
     <row r="15" spans="2:6" s="1" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="24" t="s">
@@ -1688,8 +1688,8 @@
       <c r="C19" s="29"/>
     </row>
     <row r="20" spans="2:6" ht="18" x14ac:dyDescent="0.2">
-      <c r="B20" s="81"/>
-      <c r="C20" s="81"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="86"/>
       <c r="D20" s="7"/>
       <c r="E20" s="30"/>
       <c r="F20" s="30"/>
@@ -1716,22 +1716,22 @@
       <c r="C25" s="29"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.15">
-      <c r="B26" s="82"/>
-      <c r="C26" s="82"/>
+      <c r="B26" s="87"/>
+      <c r="C26" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="C7:E7"/>
-    <mergeCell ref="C8:E8"/>
     <mergeCell ref="B14:E14"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="C9:E9"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="C7:E7"/>
+    <mergeCell ref="C8:E8"/>
   </mergeCells>
   <pageMargins left="0.5" right="0.62986111111111109" top="0.98402777777777783" bottom="0.98402777777777772" header="0.51180555555555562" footer="0.5"/>
   <pageSetup firstPageNumber="0" fitToHeight="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
@@ -1747,7 +1747,7 @@
   <dimension ref="B2:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -1816,7 +1816,7 @@
         <v>49</v>
       </c>
       <c r="E8" s="55">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="F8" s="55"/>
       <c r="G8" s="37">
@@ -1919,7 +1919,7 @@
       </c>
       <c r="E12" s="45">
         <f>SUM(E8:E10)</f>
-        <v>1257</v>
+        <v>1263</v>
       </c>
       <c r="F12" s="45" t="s">
         <v>57</v>
@@ -1983,7 +1983,7 @@
         <v>28</v>
       </c>
       <c r="C17" s="57">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="D17" s="57">
         <v>0</v>
@@ -1995,7 +1995,7 @@
         <v>0</v>
       </c>
       <c r="G17" s="57">
-        <v>453</v>
+        <v>459</v>
       </c>
       <c r="H17" s="57">
         <v>0</v>
@@ -2071,7 +2071,7 @@
       </c>
       <c r="C20" s="45">
         <f t="shared" ref="C20:H20" si="0">SUM(C17:C19)</f>
-        <v>1065</v>
+        <v>1071</v>
       </c>
       <c r="D20" s="45">
         <f t="shared" si="0"/>
@@ -2087,7 +2087,7 @@
       </c>
       <c r="G20" s="45">
         <f t="shared" si="0"/>
-        <v>1257</v>
+        <v>1263</v>
       </c>
       <c r="H20" s="45">
         <f t="shared" si="0"/>

</xml_diff>